<commit_message>
Add new item in the resource
</commit_message>
<xml_diff>
--- a/trunk/UILayout.xlsx
+++ b/trunk/UILayout.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>得分</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,12 +34,20 @@
     <t>power by lxyppc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>起点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>终点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,8 +94,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF0070C0"/>
+      <name val="华文行楷"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +152,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -151,7 +179,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -170,11 +198,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -182,23 +216,35 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -231,7 +277,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="图片 10" descr="wall.jpg"/>
+        <xdr:cNvPr id="11" name="BackGround" descr="wall.jpg" hidden="1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -271,7 +317,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="BigWall" descr="wall3.jpg"/>
+        <xdr:cNvPr id="3" name="ScoreGround" descr="wall3.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -310,7 +356,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1" descr="wall2.jpg"/>
+        <xdr:cNvPr id="2" name="PlayGround" descr="wall2.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -340,55 +386,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="184731" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6057900" y="895350"/>
-          <a:ext cx="184731" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
@@ -404,7 +401,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="Text_Next"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -484,7 +481,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvPr id="6" name="Text_Score"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -568,7 +565,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="TextBox 6"/>
+        <xdr:cNvPr id="7" name="Text_Level"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -638,71 +635,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>464343</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>351235</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>65484</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="TextBox 7"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4399359" y="1023938"/>
-          <a:ext cx="1256110" cy="589359"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
-            <a:t>power by lxyppc</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>53579</xdr:colOff>
       <xdr:row>20</xdr:row>
@@ -716,7 +648,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="TextBox 8"/>
+        <xdr:cNvPr id="9" name="Text_CopyRight"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -808,7 +740,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="TextBox 9"/>
+        <xdr:cNvPr id="10" name="NextPreview"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -873,7 +805,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="TextBox 11"/>
+        <xdr:cNvPr id="12" name="PlayGroundMask"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -919,6 +851,669 @@
         <a:lstStyle/>
         <a:p>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Text_012" hidden="1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="85725" y="1219199"/>
+          <a:ext cx="571499" cy="247651"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+              <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t>0 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+              <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+              <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t>1  2 </a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1" i="0">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Text_3" hidden="1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="542925" y="1219200"/>
+          <a:ext cx="190500" cy="247651"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+              <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t>3</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+              <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1" i="0">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Text_4689" hidden="1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="1219200"/>
+          <a:ext cx="1428750" cy="247651"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+              <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t>4 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+              <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t>   </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+              <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t> 6     8  9</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1" i="0">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Text_5" hidden="1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="819150" y="1219200"/>
+          <a:ext cx="304800" cy="247651"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+              <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t> 5 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+              <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1" i="0">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Text_7" hidden="1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1143000" y="1219200"/>
+          <a:ext cx="190500" cy="247651"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+              <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t>7</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1" i="0">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Text_GameOver"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="238125" y="1181100"/>
+          <a:ext cx="1419225" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:latin typeface="华文彩云" pitchFamily="2" charset="-122"/>
+              <a:ea typeface="华文彩云" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t>Game Over </a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1800" b="1" i="0">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:latin typeface="华文彩云" pitchFamily="2" charset="-122"/>
+            <a:ea typeface="华文彩云" pitchFamily="2" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Text_Pause"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="485776" y="1809750"/>
+          <a:ext cx="809624" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:latin typeface="Lucida Handwriting" pitchFamily="66" charset="0"/>
+              <a:ea typeface="华文彩云" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t>Pau</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:latin typeface="Lucida Handwriting" pitchFamily="66" charset="0"/>
+              <a:ea typeface="华文彩云" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t>s</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:latin typeface="Lucida Handwriting" pitchFamily="66" charset="0"/>
+              <a:ea typeface="华文彩云" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t>e</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1" i="0">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:latin typeface="Lucida Handwriting" pitchFamily="66" charset="0"/>
+            <a:ea typeface="华文彩云" pitchFamily="2" charset="-122"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Text_ScorePreview"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2162175" y="2552700"/>
+          <a:ext cx="304800" cy="247651"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+              <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t> 5 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+              <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1" i="0">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:latin typeface="华文行楷" pitchFamily="2" charset="-122"/>
+            <a:ea typeface="华文行楷" pitchFamily="2" charset="-122"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1249,17 +1844,17 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="1"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="6"/>
       <c r="S2" s="1"/>
       <c r="V2">
         <v>2</v>
@@ -1267,23 +1862,23 @@
     </row>
     <row r="3" spans="1:22" ht="13.5" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="7"/>
-      <c r="N3" s="8" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="6"/>
+      <c r="N3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
       <c r="S3" s="1"/>
       <c r="V3">
         <v>3</v>
@@ -1291,21 +1886,21 @@
     </row>
     <row r="4" spans="1:22" ht="13.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="7"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="6"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
       <c r="S4" s="1"/>
       <c r="V4">
         <v>4</v>
@@ -1313,17 +1908,17 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="1"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="6"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
@@ -1335,17 +1930,17 @@
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="1"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="6"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
@@ -1357,17 +1952,17 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="1"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="6"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
@@ -1379,17 +1974,17 @@
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="1"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="6"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
@@ -1401,17 +1996,17 @@
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="1"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="6"/>
       <c r="S9" s="1"/>
       <c r="V9">
         <v>9</v>
@@ -1419,17 +2014,17 @@
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="1"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="6"/>
       <c r="S10" s="1"/>
       <c r="V10">
         <v>10</v>
@@ -1437,23 +2032,23 @@
     </row>
     <row r="11" spans="1:22" ht="13.5" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="7"/>
-      <c r="N11" s="8" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="6"/>
+      <c r="N11" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
       <c r="S11" s="1"/>
       <c r="V11">
         <v>11</v>
@@ -1461,21 +2056,21 @@
     </row>
     <row r="12" spans="1:22" ht="13.5" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="7"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="6"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
       <c r="S12" s="1"/>
       <c r="V12">
         <v>12</v>
@@ -1483,23 +2078,23 @@
     </row>
     <row r="13" spans="1:22" ht="13.5" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
       <c r="S13" s="1"/>
       <c r="V13">
         <v>13</v>
@@ -1507,23 +2102,23 @@
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="1"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
       <c r="S14" s="1"/>
       <c r="V14">
         <v>14</v>
@@ -1531,17 +2126,17 @@
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="1"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="6"/>
       <c r="S15" s="1"/>
       <c r="V15">
         <v>15</v>
@@ -1549,17 +2144,17 @@
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="1"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="6"/>
       <c r="S16" s="1"/>
       <c r="V16">
         <v>16</v>
@@ -1567,23 +2162,23 @@
     </row>
     <row r="17" spans="1:49" ht="13.5" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="7"/>
-      <c r="N17" s="8" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="6"/>
+      <c r="N17" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
       <c r="S17" s="1"/>
       <c r="V17">
         <v>17</v>
@@ -1591,21 +2186,21 @@
     </row>
     <row r="18" spans="1:49" ht="13.5" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="7"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="6"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
       <c r="S18" s="1"/>
       <c r="V18">
         <v>18</v>
@@ -1613,19 +2208,19 @@
     </row>
     <row r="19" spans="1:49">
       <c r="A19" s="1"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="7"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="6"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
       <c r="S19" s="1"/>
       <c r="V19">
         <v>19</v>
@@ -1633,19 +2228,19 @@
     </row>
     <row r="20" spans="1:49">
       <c r="A20" s="1"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="7"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="6"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
       <c r="S20" s="1"/>
       <c r="V20">
         <v>20</v>
@@ -1653,17 +2248,17 @@
     </row>
     <row r="21" spans="1:49">
       <c r="A21" s="1"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="6"/>
       <c r="S21" s="1"/>
       <c r="V21">
         <v>21</v>
@@ -1673,21 +2268,21 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -1699,19 +2294,19 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
@@ -1777,54 +2372,54 @@
       </c>
     </row>
     <row r="27" spans="1:49">
-      <c r="P27" s="6">
+      <c r="P27" s="9">
         <f>S24</f>
         <v>19</v>
       </c>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="U27" s="6">
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="U27" s="9">
         <f>V22</f>
         <v>22</v>
       </c>
-      <c r="V27" s="6"/>
-      <c r="W27" s="6"/>
-      <c r="X27" s="6"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
     </row>
     <row r="29" spans="1:49">
-      <c r="P29" s="6">
+      <c r="P29" s="9">
         <f>P27*16</f>
         <v>304</v>
       </c>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="U29" s="6">
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="U29" s="9">
         <f>U27*16</f>
         <v>352</v>
       </c>
-      <c r="V29" s="6"/>
-      <c r="W29" s="6"/>
-      <c r="X29" s="6"/>
+      <c r="V29" s="9"/>
+      <c r="W29" s="9"/>
+      <c r="X29" s="9"/>
     </row>
     <row r="31" spans="1:49">
-      <c r="P31" s="6">
+      <c r="P31" s="9">
         <v>320</v>
       </c>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-      <c r="V31" s="6">
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="V31" s="9">
         <v>400</v>
       </c>
-      <c r="W31" s="6"/>
-      <c r="X31" s="6"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="U29:X29"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="V31:X31"/>
+    <mergeCell ref="R13:R14"/>
     <mergeCell ref="O19:O20"/>
     <mergeCell ref="P19:P20"/>
     <mergeCell ref="N3:Q4"/>
@@ -1833,11 +2428,11 @@
     <mergeCell ref="N11:Q12"/>
     <mergeCell ref="N17:Q18"/>
     <mergeCell ref="D22:P23"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="U29:X29"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="V31:X31"/>
-    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="Q13:Q14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2421,10 +3016,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA31"/>
+  <dimension ref="A1:AB31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA16" sqref="AA16"/>
+      <selection activeCell="Y32" sqref="Y32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2432,541 +3027,642 @@
     <col min="1" max="21" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="12" customHeight="1">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
+    <row r="1" spans="1:28" ht="12" customHeight="1">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="12" customHeight="1">
-      <c r="A2" s="7"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="7"/>
-      <c r="S2" s="7"/>
+    <row r="2" spans="1:28" ht="12" customHeight="1">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="6"/>
+      <c r="S2" s="6"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="12" customHeight="1">
-      <c r="A3" s="7"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="7"/>
+    <row r="3" spans="1:28" ht="12" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="6"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
       <c r="Q3" s="13"/>
-      <c r="S3" s="7"/>
+      <c r="S3" s="6"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="12" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="7"/>
+    <row r="4" spans="1:28" ht="12" customHeight="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="6"/>
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
-      <c r="S4" s="7"/>
+      <c r="S4" s="6"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="12" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="7"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="S5" s="7"/>
+    <row r="5" spans="1:28" ht="12" customHeight="1">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="6"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="S5" s="6"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="12" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="7"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="S6" s="7"/>
+    <row r="6" spans="1:28" ht="12" customHeight="1">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="6"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="S6" s="6"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
       <c r="V6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="12" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="7"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="S7" s="7"/>
+      <c r="Y6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="12" customHeight="1">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="6"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="S7" s="6"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
       <c r="V7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" ht="12" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="7"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="S8" s="7"/>
+      <c r="Y7">
+        <v>9</v>
+      </c>
+      <c r="Z7">
+        <v>9</v>
+      </c>
+      <c r="AA7">
+        <v>10</v>
+      </c>
+      <c r="AB7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="12" customHeight="1">
+      <c r="A8" s="6"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="6"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="S8" s="6"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="12" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="7"/>
-      <c r="S9" s="7"/>
+      <c r="Y8" s="8">
+        <v>3</v>
+      </c>
+      <c r="Z8">
+        <v>10</v>
+      </c>
+      <c r="AA8">
+        <v>3</v>
+      </c>
+      <c r="AB8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="12" customHeight="1">
+      <c r="A9" s="6"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="6"/>
+      <c r="S9" s="6"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="12" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="7"/>
-      <c r="S10" s="7"/>
+    <row r="10" spans="1:28" ht="12" customHeight="1">
+      <c r="A10" s="6"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="6"/>
+      <c r="S10" s="6"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" ht="12" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="7"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="S11" s="7"/>
+      <c r="Y10">
+        <f>(Y7-1)*$X$26+Y8-1</f>
+        <v>154</v>
+      </c>
+      <c r="Z10">
+        <f>(Z7-1)*$X$26+Z8-1</f>
+        <v>161</v>
+      </c>
+      <c r="AA10">
+        <f>(AA7-1)*$X$26+AA8-1</f>
+        <v>173</v>
+      </c>
+      <c r="AB10">
+        <f>(AB7-1)*$X$26+AB8-1</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="12" customHeight="1">
+      <c r="A11" s="6"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="6"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="S11" s="6"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="12" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="7"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="S12" s="7"/>
+    <row r="12" spans="1:28" ht="12" customHeight="1">
+      <c r="A12" s="6"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="6"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="S12" s="6"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="12" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="7"/>
+    <row r="13" spans="1:28" ht="12" customHeight="1">
+      <c r="A13" s="6"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="6"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" ht="12" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="7"/>
+      <c r="Y13">
+        <v>13</v>
+      </c>
+      <c r="Z13">
+        <v>13</v>
+      </c>
+      <c r="AA13">
+        <v>14</v>
+      </c>
+      <c r="AB13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="12" customHeight="1">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="6"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" ht="12" customHeight="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="7"/>
-      <c r="S15" s="7"/>
+      <c r="Y14">
+        <v>4</v>
+      </c>
+      <c r="Z14">
+        <v>9</v>
+      </c>
+      <c r="AA14">
+        <v>4</v>
+      </c>
+      <c r="AB14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="12" customHeight="1">
+      <c r="L15" s="6"/>
+      <c r="S15" s="6"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="12" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="7"/>
+    <row r="16" spans="1:28" ht="12" customHeight="1">
+      <c r="L16" s="6"/>
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
-      <c r="S16" s="7"/>
+      <c r="S16" s="6"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" ht="12" customHeight="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="7"/>
+      <c r="Y16">
+        <f>(Y13-1)*$X$26+Y14-1</f>
+        <v>231</v>
+      </c>
+      <c r="Z16">
+        <f>(Z13-1)*$X$26+Z14-1</f>
+        <v>236</v>
+      </c>
+      <c r="AA16">
+        <f>(AA13-1)*$X$26+AA14-1</f>
+        <v>250</v>
+      </c>
+      <c r="AB16">
+        <f>(AB13-1)*$X$26+AB14-1</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" ht="12" customHeight="1">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="6"/>
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
-      <c r="S17" s="7"/>
+      <c r="S17" s="6"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="12" customHeight="1">
-      <c r="A18" s="7"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="7"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="S18" s="7"/>
+    <row r="18" spans="1:28" ht="12" customHeight="1">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="6"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="S18" s="6"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" ht="12" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="7"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="S19" s="7"/>
+      <c r="X18" s="17"/>
+    </row>
+    <row r="19" spans="1:28" ht="12" customHeight="1">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="6"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="S19" s="6"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" ht="12" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="7"/>
-      <c r="S20" s="7"/>
+      <c r="Y19">
+        <v>14</v>
+      </c>
+      <c r="Z19">
+        <v>18</v>
+      </c>
+      <c r="AA19">
+        <v>19</v>
+      </c>
+      <c r="AB19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" ht="12" customHeight="1">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="6"/>
+      <c r="S20" s="6"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
       <c r="V20">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" ht="12" customHeight="1">
-      <c r="A21" s="7"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="7"/>
-      <c r="S21" s="7"/>
+      <c r="Y20">
+        <v>13</v>
+      </c>
+      <c r="Z20">
+        <v>16</v>
+      </c>
+      <c r="AA20">
+        <v>15</v>
+      </c>
+      <c r="AB20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" ht="12" customHeight="1">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="6"/>
+      <c r="S21" s="6"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
       <c r="V21">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="12" customHeight="1">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
+    <row r="22" spans="1:28" ht="12" customHeight="1">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" ht="12" customHeight="1">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
+      <c r="Y22">
+        <f>(Y19-1)*$X$26+Y20-1</f>
+        <v>259</v>
+      </c>
+      <c r="Z22">
+        <f>(Z19-1)*$X$26+Z20-1</f>
+        <v>338</v>
+      </c>
+      <c r="AA22">
+        <f>(AA19-1)*$X$26+AA20-1</f>
+        <v>356</v>
+      </c>
+      <c r="AB22">
+        <f>(AB19-1)*$X$26+AB20-1</f>
+        <v>357</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" ht="12" customHeight="1">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="12" customHeight="1">
+    <row r="24" spans="1:28" ht="12" customHeight="1">
       <c r="A24" s="2">
         <v>1</v>
       </c>
@@ -3027,7 +3723,7 @@
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:28">
       <c r="X26">
         <f>S24</f>
         <v>19</v>
@@ -3035,12 +3731,12 @@
       <c r="Z26">
         <v>23</v>
       </c>
-      <c r="AA26" s="11"/>
-    </row>
-    <row r="27" spans="1:27">
-      <c r="W27" s="11"/>
-    </row>
-    <row r="28" spans="1:27">
+      <c r="AA26" s="8"/>
+    </row>
+    <row r="27" spans="1:28">
+      <c r="W27" s="8"/>
+    </row>
+    <row r="28" spans="1:28">
       <c r="X28">
         <f>X26*16</f>
         <v>304</v>
@@ -3049,31 +3745,28 @@
         <f>Z26*16</f>
         <v>368</v>
       </c>
-      <c r="AA28" s="11"/>
-    </row>
-    <row r="29" spans="1:27">
-      <c r="W29" s="11"/>
-    </row>
-    <row r="30" spans="1:27">
+      <c r="AA28" s="8"/>
+    </row>
+    <row r="29" spans="1:28">
+      <c r="W29" s="8"/>
+    </row>
+    <row r="30" spans="1:28">
       <c r="X30">
         <v>320</v>
       </c>
       <c r="Z30">
         <v>400</v>
       </c>
-      <c r="AA30" s="11"/>
-    </row>
-    <row r="31" spans="1:27">
-      <c r="W31" s="11"/>
-      <c r="X31" s="11"/>
+      <c r="AA30" s="8"/>
+    </row>
+    <row r="31" spans="1:28">
+      <c r="W31" s="8"/>
+      <c r="X31" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="N5:Q8"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="N16:Q17"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
+  <mergeCells count="15">
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="K9:K10"/>
     <mergeCell ref="D22:P23"/>
     <mergeCell ref="N3:Q4"/>
     <mergeCell ref="N11:Q12"/>
@@ -3082,9 +3775,15 @@
     <mergeCell ref="O13:O14"/>
     <mergeCell ref="P13:P14"/>
     <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="N5:Q8"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="N16:Q17"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>